<commit_message>
Oppdaterte dokumentasjon med tidsfrister. La til tidsfrister på alle pakkeforløp i Excel
</commit_message>
<xml_diff>
--- a/doc/kreftpakkeforløp/resources/Tidsfrister_Pakkeforløp.xlsx
+++ b/doc/kreftpakkeforløp/resources/Tidsfrister_Pakkeforløp.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Tider" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tider!$A$1:$J$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tider!$A$1:$J$29</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -65,9 +65,6 @@
     <t>Blærekreft</t>
   </si>
   <si>
-    <t>Fase 3 (snitt)</t>
-  </si>
-  <si>
     <t>Kode</t>
   </si>
   <si>
@@ -225,13 +222,16 @@
   </si>
   <si>
     <t>Minste totaltid</t>
+  </si>
+  <si>
+    <t>Fase 3 (min)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,16 +247,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -264,11 +277,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,8 +306,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,7 +593,8 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +611,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -589,7 +623,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -604,12 +638,12 @@
         <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -620,8 +654,8 @@
       <c r="D2" s="1">
         <v>7</v>
       </c>
-      <c r="E2" s="1">
-        <f>MIN(G2:I2)</f>
+      <c r="E2" s="4">
+        <f>MIN(F2:H2)</f>
         <v>10</v>
       </c>
       <c r="F2" s="1">
@@ -637,10 +671,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1">
         <v>7</v>
@@ -648,8 +682,8 @@
       <c r="D3" s="1">
         <v>7</v>
       </c>
-      <c r="E3" s="1">
-        <f>MIN(G3:I3)</f>
+      <c r="E3" s="4">
+        <f>MIN(F3:H3)</f>
         <v>14</v>
       </c>
       <c r="F3" s="1">
@@ -668,31 +702,82 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
-        <v>33</v>
+      <c r="C4" s="1">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4">
+        <f>MIN(F4:H4)</f>
+        <v>8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J29" si="0">C4+D4+E4</f>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
-        <v>35</v>
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4">
+        <f>MIN(F5:H5)</f>
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
-        <v>37</v>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <f>MIN(F6:H6)</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -703,8 +788,8 @@
       <c r="D7" s="1">
         <v>14</v>
       </c>
-      <c r="E7" s="1">
-        <f>MIN(G7:I7)</f>
+      <c r="E7" s="4">
+        <f>MIN(F7:H7)</f>
         <v>3</v>
       </c>
       <c r="G7" s="1">
@@ -714,24 +799,44 @@
         <v>10</v>
       </c>
       <c r="J7" s="1">
-        <f>C7+D7+E7</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
-        <v>39</v>
+      <c r="C8" s="1">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4">
+        <f>MIN(F8:H8)</f>
+        <v>14</v>
+      </c>
+      <c r="F8" s="1">
+        <v>14</v>
+      </c>
+      <c r="G8" s="1">
+        <v>14</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1">
         <v>9</v>
@@ -739,8 +844,8 @@
       <c r="D9" s="1">
         <v>12</v>
       </c>
-      <c r="E9" s="1">
-        <f>MIN(G9:I9)</f>
+      <c r="E9" s="4">
+        <f>MIN(F9:H9)</f>
         <v>14</v>
       </c>
       <c r="F9" s="1">
@@ -753,13 +858,13 @@
         <v>18</v>
       </c>
       <c r="J9" s="1">
-        <f>C9+D9+E9</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -770,8 +875,8 @@
       <c r="D10" s="1">
         <v>25</v>
       </c>
-      <c r="E10" s="1">
-        <f>MIN(G10:I10)</f>
+      <c r="E10" s="4">
+        <f>MIN(F10:H10)</f>
         <v>14</v>
       </c>
       <c r="F10" s="1">
@@ -784,13 +889,13 @@
         <v>14</v>
       </c>
       <c r="J10" s="1">
-        <f>C10+D10+E10</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -801,8 +906,8 @@
       <c r="D11" s="1">
         <v>25</v>
       </c>
-      <c r="E11" s="1">
-        <f>MIN(G11:I11)</f>
+      <c r="E11" s="4">
+        <f>MIN(F11:H11)</f>
         <v>11</v>
       </c>
       <c r="F11" s="1">
@@ -815,16 +920,16 @@
         <v>11</v>
       </c>
       <c r="J11" s="1">
-        <f>C11+D11+E11</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1">
         <v>10</v>
@@ -832,8 +937,8 @@
       <c r="D12" s="1">
         <v>24</v>
       </c>
-      <c r="E12" s="1">
-        <f>MIN(G12:I12)</f>
+      <c r="E12" s="4">
+        <f>MIN(F12:H12)</f>
         <v>3</v>
       </c>
       <c r="F12" s="1">
@@ -846,24 +951,47 @@
         <v>32</v>
       </c>
       <c r="J12" s="1">
-        <f>C12+D12+E12</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
-        <v>43</v>
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>21</v>
+      </c>
+      <c r="E13" s="4">
+        <f>MIN(F13:H13)</f>
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <v>10</v>
+      </c>
+      <c r="G13" s="1">
+        <v>14</v>
+      </c>
+      <c r="H13" s="1">
+        <v>14</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1">
         <v>5</v>
@@ -871,8 +999,8 @@
       <c r="D14" s="1">
         <v>12</v>
       </c>
-      <c r="E14" s="1">
-        <f>MIN(G14:I14)</f>
+      <c r="E14" s="4">
+        <f>MIN(F14:H14)</f>
         <v>14</v>
       </c>
       <c r="F14" s="1">
@@ -888,16 +1016,16 @@
         <v>14</v>
       </c>
       <c r="J14" s="1">
-        <f>C14+D14+E14</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1">
         <v>6</v>
@@ -905,8 +1033,8 @@
       <c r="D15" s="1">
         <v>16</v>
       </c>
-      <c r="E15" s="1">
-        <f>MIN(G15:I15)</f>
+      <c r="E15" s="4">
+        <f>MIN(F15:H15)</f>
         <v>8</v>
       </c>
       <c r="F15" s="1">
@@ -919,16 +1047,16 @@
         <v>8</v>
       </c>
       <c r="J15" s="1">
-        <f>C15+D15+E15</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1">
         <v>6</v>
@@ -936,8 +1064,8 @@
       <c r="D16" s="1">
         <v>16</v>
       </c>
-      <c r="E16" s="1">
-        <f>MIN(G16:I16)</f>
+      <c r="E16" s="4">
+        <f>MIN(F16:H16)</f>
         <v>8</v>
       </c>
       <c r="F16" s="1">
@@ -950,16 +1078,16 @@
         <v>8</v>
       </c>
       <c r="J16" s="1">
-        <f>C16+D16+E16</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1">
         <v>6</v>
@@ -967,8 +1095,8 @@
       <c r="D17" s="1">
         <v>16</v>
       </c>
-      <c r="E17" s="1">
-        <f>MIN(G17:I17)</f>
+      <c r="E17" s="4">
+        <f>MIN(F17:H17)</f>
         <v>8</v>
       </c>
       <c r="F17" s="1">
@@ -981,21 +1109,44 @@
         <v>8</v>
       </c>
       <c r="J17" s="1">
-        <f>C17+D17+E17</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
-        <v>49</v>
+      <c r="C18" s="1">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>8</v>
+      </c>
+      <c r="E18" s="4">
+        <f>MIN(F18:H18)</f>
+        <v>7</v>
+      </c>
+      <c r="F18" s="1">
+        <v>7</v>
+      </c>
+      <c r="G18" s="1">
+        <v>14</v>
+      </c>
+      <c r="H18" s="1">
+        <v>14</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -1006,8 +1157,8 @@
       <c r="D19" s="1">
         <v>21</v>
       </c>
-      <c r="E19" s="1">
-        <f>MIN(G19:I19)</f>
+      <c r="E19" s="4">
+        <f>MIN(F19:H19)</f>
         <v>7</v>
       </c>
       <c r="F19" s="1">
@@ -1020,24 +1171,47 @@
         <v>14</v>
       </c>
       <c r="J19" s="1">
-        <f>C19+D19+E19</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
         <v>50</v>
       </c>
-      <c r="B20" t="s">
-        <v>51</v>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4">
+        <f>MIN(F20:H20)</f>
+        <v>3</v>
+      </c>
+      <c r="F20" s="1">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1">
+        <v>3</v>
+      </c>
+      <c r="H20" s="1">
+        <v>14</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1">
         <v>8</v>
@@ -1045,8 +1219,8 @@
       <c r="D21" s="1">
         <v>21</v>
       </c>
-      <c r="E21" s="1">
-        <f>MIN(G21:I21)</f>
+      <c r="E21" s="4">
+        <f>MIN(F21:H21)</f>
         <v>14</v>
       </c>
       <c r="F21" s="1">
@@ -1059,72 +1233,224 @@
         <v>14</v>
       </c>
       <c r="J21" s="1">
-        <f>C21+D21+E21</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
-        <v>54</v>
+      <c r="C22" s="1">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1">
+        <v>20</v>
+      </c>
+      <c r="E22" s="4">
+        <f>MIN(F22:H22)</f>
+        <v>7</v>
+      </c>
+      <c r="F22" s="1">
+        <v>14</v>
+      </c>
+      <c r="G22" s="1">
+        <v>7</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
         <v>55</v>
       </c>
-      <c r="B23" t="s">
-        <v>56</v>
+      <c r="C23" s="1">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1">
+        <v>21</v>
+      </c>
+      <c r="E23" s="4">
+        <f>MIN(F23:H23)</f>
+        <v>14</v>
+      </c>
+      <c r="F23" s="1">
+        <v>14</v>
+      </c>
+      <c r="G23" s="1">
+        <v>14</v>
+      </c>
+      <c r="H23" s="1">
+        <v>14</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
         <v>57</v>
       </c>
-      <c r="B24" t="s">
-        <v>58</v>
+      <c r="C24" s="1">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1">
+        <v>10</v>
+      </c>
+      <c r="E24" s="4">
+        <f>MIN(F24:H24)</f>
+        <v>21</v>
+      </c>
+      <c r="F24" s="1">
+        <v>21</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
         <v>59</v>
       </c>
-      <c r="B25" t="s">
-        <v>60</v>
+      <c r="C25" s="1">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1">
+        <v>14</v>
+      </c>
+      <c r="E25" s="4">
+        <f>MIN(F25:H25)</f>
+        <v>14</v>
+      </c>
+      <c r="F25" s="1">
+        <v>14</v>
+      </c>
+      <c r="G25" s="1">
+        <v>14</v>
+      </c>
+      <c r="H25" s="1">
+        <v>14</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
         <v>61</v>
       </c>
-      <c r="B26" t="s">
-        <v>62</v>
+      <c r="C26" s="1">
+        <v>14</v>
+      </c>
+      <c r="D26" s="1">
+        <v>21</v>
+      </c>
+      <c r="E26" s="4">
+        <f>MIN(F26:H26)</f>
+        <v>21</v>
+      </c>
+      <c r="F26" s="1">
+        <v>21</v>
+      </c>
+      <c r="G26" s="1">
+        <v>21</v>
+      </c>
+      <c r="H26" s="1">
+        <v>21</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="0"/>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
         <v>63</v>
       </c>
-      <c r="B27" t="s">
-        <v>64</v>
+      <c r="C27" s="1">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1">
+        <v>21</v>
+      </c>
+      <c r="E27" s="4">
+        <f>MIN(F27:H27)</f>
+        <v>14</v>
+      </c>
+      <c r="F27" s="1">
+        <v>21</v>
+      </c>
+      <c r="G27" s="1">
+        <v>14</v>
+      </c>
+      <c r="H27" s="1">
+        <v>21</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="s">
-        <v>30</v>
+      <c r="C28" s="1">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1">
+        <v>14</v>
+      </c>
+      <c r="E28" s="4">
+        <f>MIN(F28:H28)</f>
+        <v>10</v>
+      </c>
+      <c r="F28" s="1">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1">
+        <v>10</v>
+      </c>
+      <c r="H28" s="1">
+        <v>14</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1">
         <v>7</v>
@@ -1132,17 +1458,17 @@
       <c r="D29" s="1">
         <v>15</v>
       </c>
-      <c r="E29" s="1">
-        <f>MIN(G29:I29)</f>
+      <c r="E29" s="4">
+        <f>MIN(F29:H29)</f>
         <v>0</v>
       </c>
       <c r="J29" s="1">
-        <f>C29+D29+E29</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J10">
+  <autoFilter ref="A1:J29">
     <sortState ref="A2:J43">
       <sortCondition ref="A1:A15"/>
     </sortState>

</xml_diff>